<commit_message>
Amend pop calculation in function. Move uptake rate to before adjusting for previously screened and re-invites.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v4_test_alt.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v4_test_alt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/andy_wilson_mlcsu_nhs_uk/Documents/Git/Lung_Health_Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{6093D789-1669-4FA9-B66F-E844CFCA9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7D91E43-5CA8-4A08-8204-50FE5F85F449}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{6093D789-1669-4FA9-B66F-E844CFCA9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8146CB19-6372-4384-98C9-8A3D77667C2A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
@@ -4767,7 +4767,7 @@
   <dimension ref="B2:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4887,10 +4887,10 @@
         <v>0.15</v>
       </c>
       <c r="F6" s="10">
-        <v>0.24</v>
+        <v>0.3</v>
       </c>
       <c r="G6" s="10">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="H6" s="10">
         <v>0.75</v>

</xml_diff>

<commit_message>
Changes to the loading input and assumptions scripts.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v4_test_alt.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v4_test_alt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/andy_wilson_mlcsu_nhs_uk/Documents/Git/Lung_Health_Checks/data/config_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{6093D789-1669-4FA9-B66F-E844CFCA9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8146CB19-6372-4384-98C9-8A3D77667C2A}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{6093D789-1669-4FA9-B66F-E844CFCA9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB05EE2E-6EB3-4542-A4EA-9D563779C8D1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="6" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -1536,124 +1536,124 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="107.54296875" customWidth="1"/>
+    <col min="2" max="2" width="107.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" s="7" customFormat="1" ht="29.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:2" s="7" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="105" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:2" ht="126" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="2:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
     </row>
-    <row r="13" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B21" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B22" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B25" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B26" s="14"/>
     </row>
-    <row r="27" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
     </row>
   </sheetData>
@@ -1687,14 +1687,14 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>218</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>219</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>220</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>221</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>222</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>223</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>224</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>225</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>226</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>227</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>228</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>229</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>230</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>231</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>232</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>233</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>234</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>235</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>236</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>237</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>238</v>
       </c>
@@ -2290,15 +2290,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>60</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>62</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>146</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>174</v>
       </c>
@@ -2502,14 +2502,14 @@
       <selection activeCell="E12" sqref="E12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>155</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>156</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>84</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>157</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>159</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>86</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>88</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>89</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>90</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>91</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>158</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
@@ -2927,14 +2927,14 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>239</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>240</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>241</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>242</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>243</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>244</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>245</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>246</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>247</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>248</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>249</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>250</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>251</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>252</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>253</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>254</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>255</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>256</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>257</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>258</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>259</v>
       </c>
@@ -3530,15 +3530,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>71</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>72</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>73</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>74</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>147</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>168</v>
       </c>
@@ -3742,14 +3742,14 @@
       <selection activeCell="E12" sqref="E12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>161</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>162</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>93</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>163</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>164</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>94</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>95</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>96</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>97</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>98</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>99</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>100</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>165</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>101</v>
       </c>
@@ -4167,14 +4167,14 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>260</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>261</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>262</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>263</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>264</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>265</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>266</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>267</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>268</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>269</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>270</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>271</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>272</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>273</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>274</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>275</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>276</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>277</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>278</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>279</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>280</v>
       </c>
@@ -4766,18 +4766,18 @@
   </sheetPr>
   <dimension ref="B2:I8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4821,7 +4821,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>123</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>125</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>127</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>128</v>
       </c>
@@ -4978,14 +4978,14 @@
       <selection activeCell="E6" sqref="E6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>131</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>133</v>
       </c>
@@ -5165,14 +5165,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
@@ -5350,15 +5350,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>170</v>
       </c>
@@ -5562,14 +5562,14 @@
       <selection activeCell="E9" sqref="E9:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>139</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>142</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>49</v>
       </c>
@@ -5906,18 +5906,18 @@
   </sheetPr>
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>197</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>198</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>199</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>200</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>201</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>202</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>203</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>204</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>205</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>206</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>207</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>208</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>209</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>210</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>211</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>212</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>213</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
       <c r="F19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>2.39664469742361E-3</v>
       </c>
       <c r="G19" s="10">
         <v>2.3966446974236066E-3</v>
@@ -6385,7 +6385,7 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>214</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>215</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>216</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>217</v>
       </c>
@@ -6513,15 +6513,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>51</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>54</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>143</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>173</v>
       </c>
@@ -6725,14 +6725,14 @@
       <selection activeCell="E11" sqref="E11:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>152</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>151</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>75</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>154</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>76</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>77</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>79</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>80</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>81</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>82</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>153</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Update spelling error in excel alternate scenario spreadsheet
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v4_test_alt.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v4_test_alt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/andy_wilson_mlcsu_nhs_uk/Documents/Git/LHC_2/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{6093D789-1669-4FA9-B66F-E844CFCA9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB05EE2E-6EB3-4542-A4EA-9D563779C8D1}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{6093D789-1669-4FA9-B66F-E844CFCA9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49216D07-2219-44EC-A2E3-A8E983E35268}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="6" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="284">
   <si>
     <t>Target Lung Health Check Modelling - Model Inputs</t>
   </si>
@@ -616,9 +616,6 @@
     <t>Percentage of patients on 12 month follow-up undergoing undergoing initial diagnostics who will receive a lung function test</t>
   </si>
   <si>
-    <t>Percentage of Patients with  Coronary calcification</t>
-  </si>
-  <si>
     <t>Percentage of Number of patients with incidental findings - Emphysema (moderate or severe)</t>
   </si>
   <si>
@@ -658,9 +655,6 @@
     <t>Percentage of Patients with Pleural affusions/thickening</t>
   </si>
   <si>
-    <t>Percentage of Patients with  Suspicious Breast Legion</t>
-  </si>
-  <si>
     <t>Percentage of Patients with Consolidation</t>
   </si>
   <si>
@@ -929,6 +923,21 @@
   </si>
   <si>
     <t>m24_inc_tub</t>
+  </si>
+  <si>
+    <t>Percentage of Patients with  Suspicious Breast Lesion</t>
+  </si>
+  <si>
+    <t>Percentage of Patients with Suspicious Breast Lesion</t>
+  </si>
+  <si>
+    <t>Percentage of Patients with Coronary calcification</t>
+  </si>
+  <si>
+    <t>Percentage of Patients with Coronary calcification</t>
+  </si>
+  <si>
+    <t>Percentage of Patients with Suspicious Breast Lesion</t>
   </si>
 </sst>
 </file>
@@ -1536,124 +1545,124 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="107.5703125" customWidth="1"/>
+    <col min="2" max="2" width="107.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:2" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" s="7" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" s="7" customFormat="1" ht="29.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B7" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="126" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="105" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="15" x14ac:dyDescent="0.35">
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="15" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B12" s="14"/>
     </row>
-    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B13" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B14" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B15" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B17" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B18" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B19" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B20" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B21" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B22" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B23" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B24" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B25" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B26" s="14"/>
     </row>
-    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" ht="15" x14ac:dyDescent="0.4">
       <c r="B27" s="12"/>
     </row>
   </sheetData>
@@ -1684,17 +1693,17 @@
   <dimension ref="B2:I23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1720,12 +1729,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1746,12 +1755,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -1772,12 +1781,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1798,12 +1807,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1824,12 +1833,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -1850,12 +1859,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -1876,12 +1885,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -1902,12 +1911,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -1928,12 +1937,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -1954,12 +1963,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -1980,12 +1989,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -2006,12 +2015,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -2032,12 +2041,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -2058,12 +2067,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -2084,12 +2093,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>190</v>
+        <v>280</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -2110,12 +2119,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -2136,12 +2145,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -2162,12 +2171,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -2188,12 +2197,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -2214,12 +2223,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -2240,12 +2249,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -2268,7 +2277,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CFC3uIoapVl2QbbxmfoDQrZJkIHLMrdyZSSdwE4afSU6xW9hCzA/sdQU6Re9WvSHcS0265JaEiVKa13H0infrA==" saltValue="KO5mPCSFm3taDQOpNYlbSA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="EWc3uCyocNgByr/aCq2KYWVK9KjrM+wlJiLROu9DGIL0Kb+UxxbM+/Y+Of0Txiy7CnzO80QTfei/HuRiHDEtWw==" saltValue="0EzmCDp25jQKdZbPT4GPYQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{C2D4DCCC-2F6E-43B5-9BE7-2CCD33112B93}">
       <formula1>0</formula1>
@@ -2290,15 +2299,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2324,7 +2333,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
@@ -2350,7 +2359,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>60</v>
       </c>
@@ -2376,7 +2385,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
@@ -2402,7 +2411,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>62</v>
       </c>
@@ -2428,7 +2437,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>146</v>
       </c>
@@ -2454,7 +2463,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>174</v>
       </c>
@@ -2502,14 +2511,14 @@
       <selection activeCell="E12" sqref="E12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2535,7 +2544,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>155</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>156</v>
       </c>
@@ -2587,7 +2596,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>84</v>
       </c>
@@ -2613,7 +2622,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>157</v>
       </c>
@@ -2639,7 +2648,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>159</v>
       </c>
@@ -2665,7 +2674,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
@@ -2691,7 +2700,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>86</v>
       </c>
@@ -2717,7 +2726,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>87</v>
       </c>
@@ -2743,7 +2752,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>88</v>
       </c>
@@ -2769,7 +2778,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>89</v>
       </c>
@@ -2795,7 +2804,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>90</v>
       </c>
@@ -2821,7 +2830,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>91</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>158</v>
       </c>
@@ -2873,7 +2882,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
@@ -2923,18 +2932,18 @@
   </sheetPr>
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2960,12 +2969,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>176</v>
+        <v>281</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -2986,12 +2995,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -3012,12 +3021,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -3026,7 +3035,7 @@
         <v>2.6363091671659671E-2</v>
       </c>
       <c r="F5" s="10">
-        <v>2.6363091671659671E-2</v>
+        <v>2.6363091671659698E-2</v>
       </c>
       <c r="G5" s="10">
         <v>2.6363091671659671E-2</v>
@@ -3038,12 +3047,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -3064,12 +3073,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -3090,12 +3099,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -3116,12 +3125,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -3142,12 +3151,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -3168,12 +3177,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -3194,12 +3203,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -3220,12 +3229,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -3246,12 +3255,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -3272,12 +3281,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -3298,12 +3307,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -3324,12 +3333,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>190</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -3350,12 +3359,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -3376,12 +3385,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -3402,12 +3411,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -3428,12 +3437,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -3454,12 +3463,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -3480,12 +3489,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -3508,7 +3517,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+ZWvKlXWTnfsm2DTP6IfRHJ05lXEip04DBPLH3Jys7bFZ73f6DTzob7K+kD9nX24PBvTDQBjE+XG3xn4W9GoEg==" saltValue="4qlz4HtooLJbjcJMgEfIRQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="LhP71W/oSrK5Tg4hixGrx+/A+iJsqg+TeDEmpIKvz7yZP1nTd3+wVBqnQHAtc+WuJTXO0OUp1LqyRnvP4xQ+Rg==" saltValue="8SkbgkaNGrr+A7nSJ/++rQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{5F25A177-8CF3-40BB-8ABD-0AE9CE8F34E1}">
       <formula1>0</formula1>
@@ -3530,15 +3539,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -3564,7 +3573,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>71</v>
       </c>
@@ -3590,7 +3599,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>72</v>
       </c>
@@ -3616,7 +3625,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>73</v>
       </c>
@@ -3642,7 +3651,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>74</v>
       </c>
@@ -3668,7 +3677,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>147</v>
       </c>
@@ -3694,7 +3703,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>168</v>
       </c>
@@ -3742,14 +3751,14 @@
       <selection activeCell="E12" sqref="E12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3775,7 +3784,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>161</v>
       </c>
@@ -3801,7 +3810,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>162</v>
       </c>
@@ -3827,7 +3836,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>93</v>
       </c>
@@ -3853,7 +3862,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>163</v>
       </c>
@@ -3879,7 +3888,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>164</v>
       </c>
@@ -3905,7 +3914,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>94</v>
       </c>
@@ -3931,7 +3940,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>95</v>
       </c>
@@ -3957,7 +3966,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>96</v>
       </c>
@@ -3983,7 +3992,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>97</v>
       </c>
@@ -4009,7 +4018,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>98</v>
       </c>
@@ -4035,7 +4044,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>99</v>
       </c>
@@ -4061,7 +4070,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>100</v>
       </c>
@@ -4087,7 +4096,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>165</v>
       </c>
@@ -4113,7 +4122,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>101</v>
       </c>
@@ -4163,18 +4172,18 @@
   </sheetPr>
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -4200,12 +4209,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -4226,12 +4235,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -4252,12 +4261,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -4278,12 +4287,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -4304,12 +4313,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -4330,12 +4339,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -4356,12 +4365,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -4382,12 +4391,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -4408,12 +4417,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -4434,12 +4443,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -4460,12 +4469,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -4486,12 +4495,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -4512,12 +4521,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -4538,12 +4547,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -4564,12 +4573,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>190</v>
+        <v>283</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -4590,12 +4599,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -4616,12 +4625,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -4642,12 +4651,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -4668,12 +4677,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -4694,12 +4703,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -4720,12 +4729,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -4748,7 +4757,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ttYupC3OuY8q1gwK8w7SgS56jF8/zUrJZTfmfUMxNKeHrmy9np6dv6CX74eXRin/BBfN/Rjd/+C9ZP3+URtF4g==" saltValue="wdtPDjDskeB5Jo4viirCJA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bzfU+s5WYGtILxz2ChrBBaWTymnEWguWUg1JA0g2LQNOJv/9TmYBAmQjKNOIYkzUOOxd1L0Z0Xvp2C5pqcIkJg==" saltValue="99QgHZqhHek7K8oYtRy/HA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{4587F331-C10C-4C2C-9D6A-8C994FCBF1F2}">
       <formula1>0</formula1>
@@ -4770,14 +4779,14 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4803,7 +4812,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4821,7 +4830,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>123</v>
       </c>
@@ -4847,7 +4856,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>125</v>
       </c>
@@ -4873,7 +4882,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4899,7 +4908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>127</v>
       </c>
@@ -4925,7 +4934,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>128</v>
       </c>
@@ -4978,14 +4987,14 @@
       <selection activeCell="E6" sqref="E6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5011,7 +5020,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>131</v>
       </c>
@@ -5037,7 +5046,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -5063,7 +5072,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -5089,7 +5098,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -5115,7 +5124,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>133</v>
       </c>
@@ -5165,14 +5174,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5198,7 +5207,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
@@ -5224,7 +5233,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5250,7 +5259,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5276,7 +5285,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
@@ -5302,7 +5311,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
@@ -5350,15 +5359,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5384,7 +5393,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
@@ -5410,7 +5419,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
@@ -5436,7 +5445,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
@@ -5462,7 +5471,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
@@ -5488,7 +5497,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>137</v>
       </c>
@@ -5514,7 +5523,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>170</v>
       </c>
@@ -5562,14 +5571,14 @@
       <selection activeCell="E9" sqref="E9:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5595,7 +5604,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
@@ -5621,7 +5630,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>139</v>
       </c>
@@ -5647,7 +5656,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -5673,7 +5682,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
@@ -5699,7 +5708,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
@@ -5725,7 +5734,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
@@ -5751,7 +5760,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
@@ -5777,7 +5786,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
@@ -5803,7 +5812,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
@@ -5829,7 +5838,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>142</v>
       </c>
@@ -5855,7 +5864,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>49</v>
       </c>
@@ -5907,17 +5916,17 @@
   <dimension ref="B2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5943,12 +5952,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>176</v>
+        <v>281</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5969,12 +5978,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -5995,12 +6004,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -6021,12 +6030,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -6047,12 +6056,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -6073,12 +6082,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -6099,12 +6108,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -6125,12 +6134,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -6151,12 +6160,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -6177,12 +6186,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -6203,12 +6212,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -6229,12 +6238,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -6255,12 +6264,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -6281,12 +6290,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -6307,12 +6316,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>190</v>
+        <v>280</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -6333,12 +6342,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -6359,12 +6368,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -6385,12 +6394,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -6411,12 +6420,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -6437,12 +6446,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -6463,12 +6472,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -6491,7 +6500,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OFtf+hJd93D0Q2yffkUpVORkVz3Meq9+i10bqrItsVE07comrjDxCweO4oNZjq+yFedro+r+bsKtSDIMCLg4kg==" saltValue="AbtRUdmLv4DlreXmmjNPHA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="T1iqjREDnQYFqfMq0y0+VxiJiw8/pykqgzI8WXLmRFcCU/WCS2BNa3AlmACJDhy8rF/knoTeFCDoF4GRIM6Xmg==" saltValue="3Ei4OE9dsEI5qlylxW6bVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{96703BE1-5938-4319-9C8B-21F7C46B3A7F}">
       <formula1>0</formula1>
@@ -6513,15 +6522,15 @@
       <selection activeCell="E3" sqref="E3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -6547,7 +6556,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>51</v>
       </c>
@@ -6573,7 +6582,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
@@ -6599,7 +6608,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
@@ -6625,7 +6634,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>54</v>
       </c>
@@ -6651,7 +6660,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>143</v>
       </c>
@@ -6677,7 +6686,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>173</v>
       </c>
@@ -6722,17 +6731,17 @@
   <dimension ref="B2:I15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:I11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -6758,7 +6767,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>152</v>
       </c>
@@ -6784,7 +6793,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>151</v>
       </c>
@@ -6810,7 +6819,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>75</v>
       </c>
@@ -6836,7 +6845,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>154</v>
       </c>
@@ -6862,7 +6871,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>76</v>
       </c>
@@ -6888,7 +6897,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>77</v>
       </c>
@@ -6914,7 +6923,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
@@ -6940,7 +6949,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>79</v>
       </c>
@@ -6966,7 +6975,7 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>80</v>
       </c>
@@ -6992,7 +7001,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>81</v>
       </c>
@@ -7018,7 +7027,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>82</v>
       </c>
@@ -7044,7 +7053,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>153</v>
       </c>
@@ -7070,7 +7079,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>83</v>
       </c>

</xml_diff>